<commit_message>
Change left/right to anatomical axes orientation
Change left and right in the version ID (and therefore also in the at_id and lookup label), to the 3-letter abbreviation for the anatomical axes orientation e.g. v2004 (Bregma, right) changed into v2004 (Bregma, RIA)
</commit_message>
<xml_diff>
--- a/PaxinosWatson-RBSC/6th-edition/Pax_v6_BAV_6th_cor-Br-le.xlsx
+++ b/PaxinosWatson-RBSC/6th-edition/Pax_v6_BAV_6th_cor-Br-le.xlsx
@@ -185,9 +185,6 @@
     <t>Paxinos and Watson's Stereotaxic Rat Brain Atlas (Coronal)</t>
   </si>
   <si>
-    <t>6th ed. (Bregma, left)</t>
-  </si>
-  <si>
     <t xml:space="preserve">The 6th edition introduces color photographs of the coronal brain section. All diagrams from the previous editions have been completely revised [paraphrased from the ‘Preface’ of the book ISBN: 0-12-547612-4].  </t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>https://openminds.ebrains.eu/instances/ISBN/0-12-547612-4</t>
+  </si>
+  <si>
+    <t>6th ed. (Bregma, LIA)</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E560"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="520" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>